<commit_message>
added description to template
</commit_message>
<xml_diff>
--- a/public/web_model/template.xlsx
+++ b/public/web_model/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\stage\CRISP\public\web_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C732113F-61BC-405A-8BC0-3CD05A958C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84D21D6-B2F5-490D-A49C-9AE0B30391E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{28EB074A-B6E7-4FF4-9E0E-6C4DA293FACA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="256">
   <si>
     <t>MCV</t>
   </si>
@@ -51,33 +51,6 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>Kolom</t>
-  </si>
-  <si>
-    <t>Omschrijving</t>
-  </si>
-  <si>
-    <t>Type waarde</t>
-  </si>
-  <si>
-    <t>Alles</t>
-  </si>
-  <si>
-    <t>Nummer</t>
-  </si>
-  <si>
-    <t>0 of 1</t>
-  </si>
-  <si>
-    <t>M als Man, overige waardes zijn Vrouw</t>
-  </si>
-  <si>
-    <t>Opmerking</t>
-  </si>
-  <si>
-    <t>Zolang de kolom namen overeenkomen, maakt de volgorder niet uit.</t>
-  </si>
-  <si>
     <t>Leukocytes</t>
   </si>
   <si>
@@ -96,365 +69,749 @@
     <t>ACPA</t>
   </si>
   <si>
-    <t>s_el_left</t>
-  </si>
-  <si>
-    <t>s_pip1_left</t>
-  </si>
-  <si>
-    <t>s_pip1_right</t>
-  </si>
-  <si>
-    <t>s_ac_left</t>
-  </si>
-  <si>
-    <t>s_ac_right</t>
-  </si>
-  <si>
-    <t>s_ank_left</t>
-  </si>
-  <si>
-    <t>s_ank_right</t>
-  </si>
-  <si>
-    <t>s_dip2_left</t>
-  </si>
-  <si>
-    <t>s_dip2_right</t>
-  </si>
-  <si>
-    <t>s_dip3_left</t>
-  </si>
-  <si>
-    <t>s_dip3_right</t>
-  </si>
-  <si>
-    <t>s_dip4_left</t>
-  </si>
-  <si>
-    <t>s_dip4_right</t>
-  </si>
-  <si>
-    <t>s_dip5_left</t>
-  </si>
-  <si>
-    <t>s_dip5_right</t>
-  </si>
-  <si>
-    <t>s_el_right</t>
-  </si>
-  <si>
-    <t>s_kn_left</t>
-  </si>
-  <si>
-    <t>s_kn_right</t>
-  </si>
-  <si>
-    <t>s_mcp1_left</t>
-  </si>
-  <si>
-    <t>s_mcp1_right</t>
-  </si>
-  <si>
-    <t>s_mcp2_left</t>
-  </si>
-  <si>
-    <t>s_mcp2_right</t>
-  </si>
-  <si>
-    <t>s_mcp3_left</t>
-  </si>
-  <si>
-    <t>s_mcp3_right</t>
-  </si>
-  <si>
-    <t>s_mcp4_left</t>
-  </si>
-  <si>
-    <t>s_mcp4_right</t>
-  </si>
-  <si>
-    <t>s_mcp5_left</t>
-  </si>
-  <si>
-    <t>s_mcp5_right</t>
-  </si>
-  <si>
-    <t>s_mtp1_left</t>
-  </si>
-  <si>
-    <t>s_mtp1_right</t>
-  </si>
-  <si>
-    <t>s_mtp2_left</t>
-  </si>
-  <si>
-    <t>s_mtp2_right</t>
-  </si>
-  <si>
-    <t>s_mtp3_left</t>
-  </si>
-  <si>
-    <t>s_mtp3_right</t>
-  </si>
-  <si>
-    <t>s_mtp4_left</t>
-  </si>
-  <si>
-    <t>s_mtp4_right</t>
-  </si>
-  <si>
-    <t>s_mtp5_left</t>
-  </si>
-  <si>
-    <t>s_mtp5_right</t>
-  </si>
-  <si>
     <t>s_onderste_spronggewricht_left</t>
   </si>
   <si>
     <t>s_onderste_spronggewricht_right</t>
   </si>
   <si>
-    <t>s_pip2_left</t>
-  </si>
-  <si>
-    <t>s_pip2_right</t>
-  </si>
-  <si>
-    <t>s_pip3_left</t>
-  </si>
-  <si>
-    <t>s_pip3_right</t>
-  </si>
-  <si>
-    <t>s_pip4_left</t>
-  </si>
-  <si>
-    <t>s_pip4_right</t>
-  </si>
-  <si>
-    <t>s_pip5_left</t>
-  </si>
-  <si>
-    <t>s_pip5_right</t>
-  </si>
-  <si>
-    <t>s_wr_left</t>
-  </si>
-  <si>
-    <t>s_wr_right</t>
-  </si>
-  <si>
-    <t>s_sh_left</t>
-  </si>
-  <si>
-    <t>s_sh_right</t>
-  </si>
-  <si>
-    <t>s_sc_left</t>
-  </si>
-  <si>
-    <t>s_sc_right</t>
-  </si>
-  <si>
-    <t>s_tar_left</t>
-  </si>
-  <si>
-    <t>s_tar_right</t>
-  </si>
-  <si>
-    <t>s_tm_left</t>
-  </si>
-  <si>
-    <t>s_tm_right</t>
-  </si>
-  <si>
-    <t>t_el_left</t>
-  </si>
-  <si>
-    <t>t_pip1_left</t>
-  </si>
-  <si>
-    <t>t_pip1_right</t>
-  </si>
-  <si>
-    <t>t_ac_left</t>
-  </si>
-  <si>
-    <t>t_ac_right</t>
-  </si>
-  <si>
-    <t>t_ank_left</t>
-  </si>
-  <si>
-    <t>t_ank_right</t>
-  </si>
-  <si>
-    <t>t_dip2_left</t>
-  </si>
-  <si>
-    <t>t_dip2_right</t>
-  </si>
-  <si>
-    <t>t_dip3_left</t>
-  </si>
-  <si>
-    <t>t_dip3_right</t>
-  </si>
-  <si>
-    <t>t_dip4_left</t>
-  </si>
-  <si>
-    <t>t_dip4_right</t>
-  </si>
-  <si>
-    <t>t_dip5_left</t>
-  </si>
-  <si>
-    <t>t_dip5_right</t>
-  </si>
-  <si>
-    <t>t_el_right</t>
-  </si>
-  <si>
-    <t>t_hip_left</t>
-  </si>
-  <si>
-    <t>t_hip_right</t>
-  </si>
-  <si>
-    <t>t_kn_left</t>
-  </si>
-  <si>
-    <t>t_kn_right</t>
-  </si>
-  <si>
-    <t>t_mcp1_left</t>
-  </si>
-  <si>
-    <t>t_mcp1_right</t>
-  </si>
-  <si>
-    <t>t_mcp2_left</t>
-  </si>
-  <si>
-    <t>t_mcp2_right</t>
-  </si>
-  <si>
-    <t>t_mcp3_left</t>
-  </si>
-  <si>
-    <t>t_mcp3_right</t>
-  </si>
-  <si>
-    <t>t_mcp4_left</t>
-  </si>
-  <si>
-    <t>t_mcp4_right</t>
-  </si>
-  <si>
-    <t>t_mcp5_left</t>
-  </si>
-  <si>
-    <t>t_mcp5_right</t>
-  </si>
-  <si>
-    <t>t_mtp1_left</t>
-  </si>
-  <si>
-    <t>t_mtp1_right</t>
-  </si>
-  <si>
-    <t>t_mtp2_left</t>
-  </si>
-  <si>
-    <t>t_mtp2_right</t>
-  </si>
-  <si>
-    <t>t_mtp3_left</t>
-  </si>
-  <si>
-    <t>t_mtp3_right</t>
-  </si>
-  <si>
-    <t>t_mtp4_left</t>
-  </si>
-  <si>
-    <t>t_mtp4_right</t>
-  </si>
-  <si>
-    <t>t_mtp5_left</t>
-  </si>
-  <si>
-    <t>t_mtp5_right</t>
-  </si>
-  <si>
     <t>t_onderste_spronggewricht_left</t>
   </si>
   <si>
     <t>t_onderste_spronggewricht_right</t>
   </si>
   <si>
-    <t>t_pip2_left</t>
-  </si>
-  <si>
-    <t>t_pip2_right</t>
-  </si>
-  <si>
-    <t>t_pip3_left</t>
-  </si>
-  <si>
-    <t>t_pip3_right</t>
-  </si>
-  <si>
-    <t>t_pip4_left</t>
-  </si>
-  <si>
-    <t>t_pip4_right</t>
-  </si>
-  <si>
-    <t>t_pip5_left</t>
-  </si>
-  <si>
-    <t>t_pip5_right</t>
-  </si>
-  <si>
-    <t>t_wr_left</t>
-  </si>
-  <si>
-    <t>t_wr_right</t>
-  </si>
-  <si>
-    <t>t_sh_left</t>
-  </si>
-  <si>
-    <t>t_sh_right</t>
-  </si>
-  <si>
-    <t>t_sc_left</t>
-  </si>
-  <si>
-    <t>t_sc_right</t>
-  </si>
-  <si>
-    <t>t_tar_left</t>
-  </si>
-  <si>
-    <t>t_tar_right</t>
-  </si>
-  <si>
-    <t>t_tm_left</t>
-  </si>
-  <si>
-    <t>t_tm_right</t>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>The column names are case-sensitive</t>
+  </si>
+  <si>
+    <t>The order doesn't matter</t>
+  </si>
+  <si>
+    <t>Everything</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>0, 1</t>
+  </si>
+  <si>
+    <t>M if male, everything else is female</t>
+  </si>
+  <si>
+    <t>Mean corpuscular volume</t>
+  </si>
+  <si>
+    <t>Erythrocyte sedimentation rate</t>
+  </si>
+  <si>
+    <t>Rheumatoid factor</t>
+  </si>
+  <si>
+    <t>Anti-cyclic citrullinated peptide (ccp) antibodies</t>
+  </si>
+  <si>
+    <t>s_ac_left </t>
+  </si>
+  <si>
+    <t>Swollen Acromioclavicular Left  </t>
+  </si>
+  <si>
+    <t>s_ac_right </t>
+  </si>
+  <si>
+    <t>Swollen Acromioclavicular Right </t>
+  </si>
+  <si>
+    <t>s_ank_left </t>
+  </si>
+  <si>
+    <t>Swollen Ankle Left  </t>
+  </si>
+  <si>
+    <t>s_ank_right </t>
+  </si>
+  <si>
+    <t>Swollen Ankle Right </t>
+  </si>
+  <si>
+    <t>s_dip2_left </t>
+  </si>
+  <si>
+    <t>Swollen Distal Interphalangeal II Left  </t>
+  </si>
+  <si>
+    <t>s_dip2_right </t>
+  </si>
+  <si>
+    <t>Swollen Distal Interphalangeal II Right </t>
+  </si>
+  <si>
+    <t>s_dip3_left </t>
+  </si>
+  <si>
+    <t>Swollen Distal Interphalangeal III Left  </t>
+  </si>
+  <si>
+    <t>s_dip3_right </t>
+  </si>
+  <si>
+    <t>Swollen Distal Interphalangeal III Right </t>
+  </si>
+  <si>
+    <t>s_dip4_left </t>
+  </si>
+  <si>
+    <t>Swollen Distal Interphalangeal IV Left  </t>
+  </si>
+  <si>
+    <t>s_dip4_right </t>
+  </si>
+  <si>
+    <t>Swollen Distal Interphalangeal IV Right </t>
+  </si>
+  <si>
+    <t>s_dip5_left </t>
+  </si>
+  <si>
+    <t>Swollen Distal Interphalangeal V Left  </t>
+  </si>
+  <si>
+    <t>s_dip5_right </t>
+  </si>
+  <si>
+    <t>Swollen Distal Interphalangeal V Right </t>
+  </si>
+  <si>
+    <t>s_el_left </t>
+  </si>
+  <si>
+    <t>Swollen Elbow Left  </t>
+  </si>
+  <si>
+    <t>s_el_right </t>
+  </si>
+  <si>
+    <t>Swollen Elbow Right </t>
+  </si>
+  <si>
+    <t>s_kn_left </t>
+  </si>
+  <si>
+    <t>Swollen Knee Left  </t>
+  </si>
+  <si>
+    <t>s_kn_right </t>
+  </si>
+  <si>
+    <t>Swollen Knee Right </t>
+  </si>
+  <si>
+    <t>s_mcp1_left </t>
+  </si>
+  <si>
+    <t>Swollen Metacarpophalangeal  I Left  </t>
+  </si>
+  <si>
+    <t>s_mcp1_right </t>
+  </si>
+  <si>
+    <t>Swollen Metacarpophalangeal  I Right </t>
+  </si>
+  <si>
+    <t>s_mcp2_left </t>
+  </si>
+  <si>
+    <t>Swollen Metacarpophalangeal  II Left  </t>
+  </si>
+  <si>
+    <t>s_mcp2_right </t>
+  </si>
+  <si>
+    <t>Swollen Metacarpophalangeal  II Right </t>
+  </si>
+  <si>
+    <t>s_mcp3_left </t>
+  </si>
+  <si>
+    <t>Swollen Metacarpophalangeal  III Left  </t>
+  </si>
+  <si>
+    <t>s_mcp3_right </t>
+  </si>
+  <si>
+    <t>Swollen Metacarpophalangeal  III Right </t>
+  </si>
+  <si>
+    <t>s_mcp4_left </t>
+  </si>
+  <si>
+    <t>Swollen Metacarpophalangeal  IV Left  </t>
+  </si>
+  <si>
+    <t>s_mcp4_right </t>
+  </si>
+  <si>
+    <t>Swollen Metacarpophalangeal  IV Right </t>
+  </si>
+  <si>
+    <t>s_mcp5_left </t>
+  </si>
+  <si>
+    <t>Swollen Metacarpophalangeal  V Left  </t>
+  </si>
+  <si>
+    <t>s_mcp5_right </t>
+  </si>
+  <si>
+    <t>Swollen Metacarpophalangeal  V Right </t>
+  </si>
+  <si>
+    <t>s_mtp1_left </t>
+  </si>
+  <si>
+    <t>Swollen Metatarsophalangeal I Left  </t>
+  </si>
+  <si>
+    <t>s_mtp1_right </t>
+  </si>
+  <si>
+    <t>Swollen Metatarsophalangeal I Right </t>
+  </si>
+  <si>
+    <t>s_mtp2_left </t>
+  </si>
+  <si>
+    <t>Swollen Metatarsophalangeal II Left  </t>
+  </si>
+  <si>
+    <t>s_mtp2_right </t>
+  </si>
+  <si>
+    <t>Swollen Metatarsophalangeal II Right </t>
+  </si>
+  <si>
+    <t>s_mtp3_left </t>
+  </si>
+  <si>
+    <t>Swollen Metatarsophalangeal III Left  </t>
+  </si>
+  <si>
+    <t>s_mtp3_right </t>
+  </si>
+  <si>
+    <t>Swollen Metatarsophalangeal III Right </t>
+  </si>
+  <si>
+    <t>s_mtp4_left </t>
+  </si>
+  <si>
+    <t>Swollen Metatarsophalangeal IV Left  </t>
+  </si>
+  <si>
+    <t>s_mtp4_right </t>
+  </si>
+  <si>
+    <t>Swollen Metatarsophalangeal IV Right </t>
+  </si>
+  <si>
+    <t>s_mtp5_left </t>
+  </si>
+  <si>
+    <t>Swollen Metatarsophalangeal V Left  </t>
+  </si>
+  <si>
+    <t>s_mtp5_right </t>
+  </si>
+  <si>
+    <t>Swollen Metatarsophalangeal V Right </t>
+  </si>
+  <si>
+    <t>s_pip1_left </t>
+  </si>
+  <si>
+    <t>Swollen Proximal Interphalangeal I Thumb Left  </t>
+  </si>
+  <si>
+    <t>s_pip1_right </t>
+  </si>
+  <si>
+    <t>Swollen Proximal Interphalangeal I Thumb Right </t>
+  </si>
+  <si>
+    <t>s_pip2_left </t>
+  </si>
+  <si>
+    <t>Swollen Proximal Interphalangeal II Left  </t>
+  </si>
+  <si>
+    <t>s_pip2_right </t>
+  </si>
+  <si>
+    <t>Swollen Proximal Interphalangeal II Right </t>
+  </si>
+  <si>
+    <t>s_pip3_left </t>
+  </si>
+  <si>
+    <t>Swollen Proximal Interphalangeal III Left  </t>
+  </si>
+  <si>
+    <t>s_pip3_right </t>
+  </si>
+  <si>
+    <t>Swollen Proximal Interphalangeal III Right </t>
+  </si>
+  <si>
+    <t>s_pip4_left </t>
+  </si>
+  <si>
+    <t>Swollen Proximal Interphalangeal IV Left  </t>
+  </si>
+  <si>
+    <t>s_pip4_right </t>
+  </si>
+  <si>
+    <t>Swollen Proximal Interphalangeal IV Right </t>
+  </si>
+  <si>
+    <t>s_pip5_left </t>
+  </si>
+  <si>
+    <t>Swollen Proximal Interphalangeal V Left  </t>
+  </si>
+  <si>
+    <t>s_pip5_right </t>
+  </si>
+  <si>
+    <t>Swollen Proximal Interphalangeal V Right </t>
+  </si>
+  <si>
+    <t>s_sc_left </t>
+  </si>
+  <si>
+    <t>Swollen Sternoclavicular Left  </t>
+  </si>
+  <si>
+    <t>s_sc_right </t>
+  </si>
+  <si>
+    <t>Swollen Sternoclavicular Right </t>
+  </si>
+  <si>
+    <t>s_sh_left </t>
+  </si>
+  <si>
+    <t>Swollen Shoulder Left  </t>
+  </si>
+  <si>
+    <t>s_sh_right </t>
+  </si>
+  <si>
+    <t>Swollen Shoulder Right </t>
+  </si>
+  <si>
+    <t>s_tar_left </t>
+  </si>
+  <si>
+    <t>Swollen Tarsus Left  </t>
+  </si>
+  <si>
+    <t>s_tar_right </t>
+  </si>
+  <si>
+    <t>Swollen Tarsus Right </t>
+  </si>
+  <si>
+    <t>s_tm_left </t>
+  </si>
+  <si>
+    <t>Swollen Temporomandibular Left  </t>
+  </si>
+  <si>
+    <t>s_tm_right </t>
+  </si>
+  <si>
+    <t>Swollen Temporomandibular Right </t>
+  </si>
+  <si>
+    <t>s_wr_left </t>
+  </si>
+  <si>
+    <t>Swollen Wrist Left  </t>
+  </si>
+  <si>
+    <t>s_wr_right </t>
+  </si>
+  <si>
+    <t>Swollen Wrist Right </t>
+  </si>
+  <si>
+    <t>t_ac_left </t>
+  </si>
+  <si>
+    <t>Tender Acromioclavicular Left  </t>
+  </si>
+  <si>
+    <t>t_ac_right </t>
+  </si>
+  <si>
+    <t>Tender Acromioclavicular Right </t>
+  </si>
+  <si>
+    <t>t_ank_left </t>
+  </si>
+  <si>
+    <t>Tender Ankle Left  </t>
+  </si>
+  <si>
+    <t>t_ank_right </t>
+  </si>
+  <si>
+    <t>Tender Ankle Right </t>
+  </si>
+  <si>
+    <t>t_dip2_left </t>
+  </si>
+  <si>
+    <t>Tender Distal Interphalangeal II Left  </t>
+  </si>
+  <si>
+    <t>t_dip2_right </t>
+  </si>
+  <si>
+    <t>Tender Distal Interphalangeal II Right </t>
+  </si>
+  <si>
+    <t>t_dip3_left </t>
+  </si>
+  <si>
+    <t>Tender Distal Interphalangeal III Left  </t>
+  </si>
+  <si>
+    <t>t_dip3_right </t>
+  </si>
+  <si>
+    <t>Tender Distal Interphalangeal III Right </t>
+  </si>
+  <si>
+    <t>t_dip4_left </t>
+  </si>
+  <si>
+    <t>Tender Distal Interphalangeal IV Left  </t>
+  </si>
+  <si>
+    <t>t_dip4_right </t>
+  </si>
+  <si>
+    <t>Tender Distal Interphalangeal IV Right </t>
+  </si>
+  <si>
+    <t>t_dip5_left </t>
+  </si>
+  <si>
+    <t>Tender Distal Interphalangeal V Left  </t>
+  </si>
+  <si>
+    <t>t_dip5_right </t>
+  </si>
+  <si>
+    <t>Tender Distal Interphalangeal V Right </t>
+  </si>
+  <si>
+    <t>t_el_left </t>
+  </si>
+  <si>
+    <t>Tender Elbow Left  </t>
+  </si>
+  <si>
+    <t>t_el_right </t>
+  </si>
+  <si>
+    <t>Tender Elbow Right </t>
+  </si>
+  <si>
+    <t>t_hip_left </t>
+  </si>
+  <si>
+    <t>Tender Hip Left  </t>
+  </si>
+  <si>
+    <t>t_hip_right </t>
+  </si>
+  <si>
+    <t>Tender Hip Right </t>
+  </si>
+  <si>
+    <t>t_ip1_left </t>
+  </si>
+  <si>
+    <t>Tender Interphalangeal I Great Toe Left  </t>
+  </si>
+  <si>
+    <t>t_ip1_right </t>
+  </si>
+  <si>
+    <t>Tender Interphalangeal I Great Toe Right </t>
+  </si>
+  <si>
+    <t>t_ip2_left </t>
+  </si>
+  <si>
+    <t>Tender Interphalangeal II Left  </t>
+  </si>
+  <si>
+    <t>t_ip2_right </t>
+  </si>
+  <si>
+    <t>Tender Interphalangeal II Right </t>
+  </si>
+  <si>
+    <t>t_ip3_left </t>
+  </si>
+  <si>
+    <t>Tender Interphalangeal III Left  </t>
+  </si>
+  <si>
+    <t>t_ip3_right </t>
+  </si>
+  <si>
+    <t>Tender Interphalangeal III Right </t>
+  </si>
+  <si>
+    <t>t_ip4_left </t>
+  </si>
+  <si>
+    <t>Tender Interphalangeal IV Left  </t>
+  </si>
+  <si>
+    <t>t_ip4_right </t>
+  </si>
+  <si>
+    <t>Tender Interphalangeal IV Right </t>
+  </si>
+  <si>
+    <t>t_ip5_left </t>
+  </si>
+  <si>
+    <t>Tender Interphalangeal V Left  </t>
+  </si>
+  <si>
+    <t>t_ip5_right </t>
+  </si>
+  <si>
+    <t>Tender Interphalangeal V Right </t>
+  </si>
+  <si>
+    <t>t_kn_left </t>
+  </si>
+  <si>
+    <t>Tender Knee Left  </t>
+  </si>
+  <si>
+    <t>t_kn_right </t>
+  </si>
+  <si>
+    <t>Tender Knee Right </t>
+  </si>
+  <si>
+    <t>t_mcp1_left </t>
+  </si>
+  <si>
+    <t>Tender Metacarpophalangeal  I Left  </t>
+  </si>
+  <si>
+    <t>t_mcp1_right </t>
+  </si>
+  <si>
+    <t>Tender Metacarpophalangeal  I Right </t>
+  </si>
+  <si>
+    <t>t_mcp2_left </t>
+  </si>
+  <si>
+    <t>Tender Metacarpophalangeal  II Left  </t>
+  </si>
+  <si>
+    <t>t_mcp2_right </t>
+  </si>
+  <si>
+    <t>Tender Metacarpophalangeal  II Right </t>
+  </si>
+  <si>
+    <t>t_mcp3_left </t>
+  </si>
+  <si>
+    <t>Tender Metacarpophalangeal  III Left  </t>
+  </si>
+  <si>
+    <t>t_mcp3_right </t>
+  </si>
+  <si>
+    <t>Tender Metacarpophalangeal  III Right </t>
+  </si>
+  <si>
+    <t>t_mcp4_left </t>
+  </si>
+  <si>
+    <t>Tender Metacarpophalangeal  IV Left  </t>
+  </si>
+  <si>
+    <t>t_mcp4_right </t>
+  </si>
+  <si>
+    <t>Tender Metacarpophalangeal  IV Right </t>
+  </si>
+  <si>
+    <t>t_mcp5_left </t>
+  </si>
+  <si>
+    <t>Tender Metacarpophalangeal  V Left  </t>
+  </si>
+  <si>
+    <t>t_mcp5_right </t>
+  </si>
+  <si>
+    <t>Tender Metacarpophalangeal  V Right </t>
+  </si>
+  <si>
+    <t>t_pip1_left </t>
+  </si>
+  <si>
+    <t>Tender Proximal Interphalangeal I Thumb Left  </t>
+  </si>
+  <si>
+    <t>t_pip1_right </t>
+  </si>
+  <si>
+    <t>Tender Proximal Interphalangeal I Thumb Right </t>
+  </si>
+  <si>
+    <t>t_pip2_left </t>
+  </si>
+  <si>
+    <t>Tender Proximal Interphalangeal II Left  </t>
+  </si>
+  <si>
+    <t>t_pip2_right </t>
+  </si>
+  <si>
+    <t>Tender Proximal Interphalangeal II Right </t>
+  </si>
+  <si>
+    <t>t_pip3_left </t>
+  </si>
+  <si>
+    <t>Tender Proximal Interphalangeal III Left  </t>
+  </si>
+  <si>
+    <t>t_pip3_right </t>
+  </si>
+  <si>
+    <t>Tender Proximal Interphalangeal III Right </t>
+  </si>
+  <si>
+    <t>t_pip4_left </t>
+  </si>
+  <si>
+    <t>Tender Proximal Interphalangeal IV Left  </t>
+  </si>
+  <si>
+    <t>t_pip4_right </t>
+  </si>
+  <si>
+    <t>Tender Proximal Interphalangeal IV Right </t>
+  </si>
+  <si>
+    <t>t_pip5_left </t>
+  </si>
+  <si>
+    <t>Tender Proximal Interphalangeal V Left  </t>
+  </si>
+  <si>
+    <t>t_pip5_right </t>
+  </si>
+  <si>
+    <t>Tender Proximal Interphalangeal V Right </t>
+  </si>
+  <si>
+    <t>t_sc_left </t>
+  </si>
+  <si>
+    <t>Tender sternoclavicular Left  </t>
+  </si>
+  <si>
+    <t>t_sc_right </t>
+  </si>
+  <si>
+    <t>Tender Sternoclavicular Right </t>
+  </si>
+  <si>
+    <t>t_sh_left </t>
+  </si>
+  <si>
+    <t>Tender Shoulder Left  </t>
+  </si>
+  <si>
+    <t>t_sh_right </t>
+  </si>
+  <si>
+    <t>Tender Shoulder Right </t>
+  </si>
+  <si>
+    <t>t_tar_left </t>
+  </si>
+  <si>
+    <t>Tender Tarsus Left  </t>
+  </si>
+  <si>
+    <t>t_tar_right </t>
+  </si>
+  <si>
+    <t>Tender Tarsus Right </t>
+  </si>
+  <si>
+    <t>t_tm_left </t>
+  </si>
+  <si>
+    <t>Tender Temporomandibular Left  </t>
+  </si>
+  <si>
+    <t>t_tm_right </t>
+  </si>
+  <si>
+    <t>Tender Temporomandibular Right </t>
+  </si>
+  <si>
+    <t>t_wr_left </t>
+  </si>
+  <si>
+    <t>Tender Wrist Left  </t>
+  </si>
+  <si>
+    <t>t_wr_right </t>
+  </si>
+  <si>
+    <t>Tender Wrist Right </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,13 +833,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -497,9 +866,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -847,68 +1218,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,23 +1296,29 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -940,956 +1326,1303 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>82</v>
+      </c>
+      <c r="B39" t="s">
+        <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>88</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>94</v>
+      </c>
+      <c r="B45" t="s">
+        <v>95</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>96</v>
+      </c>
+      <c r="B46" t="s">
+        <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>55</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B48" s="3"/>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>56</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B49" s="3"/>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>104</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>106</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
       </c>
       <c r="C54" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>110</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>112</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>114</v>
+      </c>
+      <c r="B57" t="s">
+        <v>115</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>118</v>
+      </c>
+      <c r="B59" t="s">
+        <v>119</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
       </c>
       <c r="C60" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>122</v>
+      </c>
+      <c r="B61" t="s">
+        <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>124</v>
+      </c>
+      <c r="B62" t="s">
+        <v>125</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
+        <v>127</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>128</v>
+      </c>
+      <c r="B64" t="s">
+        <v>129</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>72</v>
+        <v>130</v>
+      </c>
+      <c r="B65" t="s">
+        <v>131</v>
       </c>
       <c r="C65" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>132</v>
+      </c>
+      <c r="B66" t="s">
+        <v>133</v>
       </c>
       <c r="C66" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>134</v>
+      </c>
+      <c r="B67" t="s">
+        <v>135</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>136</v>
+      </c>
+      <c r="B68" t="s">
+        <v>137</v>
       </c>
       <c r="C68" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>138</v>
+      </c>
+      <c r="B69" t="s">
+        <v>139</v>
       </c>
       <c r="C69" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>77</v>
+        <v>140</v>
+      </c>
+      <c r="B70" t="s">
+        <v>141</v>
       </c>
       <c r="C70" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>142</v>
+      </c>
+      <c r="B71" t="s">
+        <v>143</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>144</v>
+      </c>
+      <c r="B72" t="s">
+        <v>145</v>
       </c>
       <c r="C72" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>146</v>
+      </c>
+      <c r="B73" t="s">
+        <v>147</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>81</v>
+        <v>148</v>
+      </c>
+      <c r="B74" t="s">
+        <v>149</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>82</v>
+        <v>150</v>
+      </c>
+      <c r="B75" t="s">
+        <v>151</v>
       </c>
       <c r="C75" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>83</v>
+        <v>152</v>
+      </c>
+      <c r="B76" t="s">
+        <v>153</v>
       </c>
       <c r="C76" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>84</v>
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
+        <v>155</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>156</v>
+      </c>
+      <c r="B78" t="s">
+        <v>157</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>158</v>
+      </c>
+      <c r="B79" t="s">
+        <v>159</v>
       </c>
       <c r="C79" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>87</v>
+        <v>160</v>
+      </c>
+      <c r="B80" t="s">
+        <v>161</v>
       </c>
       <c r="C80" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>162</v>
+      </c>
+      <c r="B81" t="s">
+        <v>163</v>
       </c>
       <c r="C81" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>164</v>
+      </c>
+      <c r="B82" t="s">
+        <v>165</v>
       </c>
       <c r="C82" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>166</v>
+      </c>
+      <c r="B83" t="s">
+        <v>167</v>
       </c>
       <c r="C83" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>168</v>
+      </c>
+      <c r="B84" t="s">
+        <v>169</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>92</v>
+        <v>170</v>
+      </c>
+      <c r="B85" t="s">
+        <v>171</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>172</v>
+      </c>
+      <c r="B86" t="s">
+        <v>173</v>
       </c>
       <c r="C86" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>174</v>
+      </c>
+      <c r="B87" t="s">
+        <v>175</v>
       </c>
       <c r="C87" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>176</v>
+      </c>
+      <c r="B88" t="s">
+        <v>177</v>
       </c>
       <c r="C88" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>178</v>
+      </c>
+      <c r="B89" t="s">
+        <v>179</v>
       </c>
       <c r="C89" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>180</v>
+      </c>
+      <c r="B90" t="s">
+        <v>181</v>
       </c>
       <c r="C90" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>182</v>
+      </c>
+      <c r="B91" t="s">
+        <v>183</v>
       </c>
       <c r="C91" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>99</v>
+        <v>184</v>
+      </c>
+      <c r="B92" t="s">
+        <v>185</v>
       </c>
       <c r="C92" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>100</v>
+        <v>186</v>
+      </c>
+      <c r="B93" t="s">
+        <v>187</v>
       </c>
       <c r="C93" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>101</v>
+        <v>188</v>
+      </c>
+      <c r="B94" t="s">
+        <v>189</v>
       </c>
       <c r="C94" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>102</v>
+        <v>190</v>
+      </c>
+      <c r="B95" t="s">
+        <v>191</v>
       </c>
       <c r="C95" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>103</v>
+        <v>192</v>
+      </c>
+      <c r="B96" t="s">
+        <v>193</v>
       </c>
       <c r="C96" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>104</v>
+        <v>194</v>
+      </c>
+      <c r="B97" t="s">
+        <v>195</v>
       </c>
       <c r="C97" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>105</v>
+        <v>196</v>
+      </c>
+      <c r="B98" t="s">
+        <v>197</v>
       </c>
       <c r="C98" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>106</v>
+        <v>198</v>
+      </c>
+      <c r="B99" t="s">
+        <v>199</v>
       </c>
       <c r="C99" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>107</v>
+        <v>200</v>
+      </c>
+      <c r="B100" t="s">
+        <v>201</v>
       </c>
       <c r="C100" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>108</v>
+        <v>202</v>
+      </c>
+      <c r="B101" t="s">
+        <v>203</v>
       </c>
       <c r="C101" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>109</v>
+        <v>204</v>
+      </c>
+      <c r="B102" t="s">
+        <v>205</v>
       </c>
       <c r="C102" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>110</v>
+        <v>206</v>
+      </c>
+      <c r="B103" t="s">
+        <v>207</v>
       </c>
       <c r="C103" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>111</v>
+        <v>208</v>
+      </c>
+      <c r="B104" t="s">
+        <v>209</v>
       </c>
       <c r="C104" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>112</v>
+        <v>210</v>
+      </c>
+      <c r="B105" t="s">
+        <v>211</v>
       </c>
       <c r="C105" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>113</v>
+        <v>212</v>
+      </c>
+      <c r="B106" t="s">
+        <v>213</v>
       </c>
       <c r="C106" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>114</v>
+        <v>214</v>
+      </c>
+      <c r="B107" t="s">
+        <v>215</v>
       </c>
       <c r="C107" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>115</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B108" s="3"/>
       <c r="C108" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>116</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B109" s="3"/>
       <c r="C109" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>117</v>
+        <v>216</v>
+      </c>
+      <c r="B110" t="s">
+        <v>217</v>
       </c>
       <c r="C110" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>118</v>
+        <v>218</v>
+      </c>
+      <c r="B111" t="s">
+        <v>219</v>
       </c>
       <c r="C111" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>119</v>
+        <v>220</v>
+      </c>
+      <c r="B112" t="s">
+        <v>221</v>
       </c>
       <c r="C112" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>120</v>
+        <v>222</v>
+      </c>
+      <c r="B113" t="s">
+        <v>223</v>
       </c>
       <c r="C113" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>121</v>
+        <v>224</v>
+      </c>
+      <c r="B114" t="s">
+        <v>225</v>
       </c>
       <c r="C114" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>122</v>
+        <v>226</v>
+      </c>
+      <c r="B115" t="s">
+        <v>227</v>
       </c>
       <c r="C115" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>123</v>
+        <v>228</v>
+      </c>
+      <c r="B116" t="s">
+        <v>229</v>
       </c>
       <c r="C116" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>124</v>
+        <v>230</v>
+      </c>
+      <c r="B117" t="s">
+        <v>231</v>
       </c>
       <c r="C117" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>125</v>
+        <v>232</v>
+      </c>
+      <c r="B118" t="s">
+        <v>233</v>
       </c>
       <c r="C118" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>126</v>
+        <v>234</v>
+      </c>
+      <c r="B119" t="s">
+        <v>235</v>
       </c>
       <c r="C119" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>127</v>
+        <v>236</v>
+      </c>
+      <c r="B120" t="s">
+        <v>237</v>
       </c>
       <c r="C120" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>128</v>
+        <v>238</v>
+      </c>
+      <c r="B121" t="s">
+        <v>239</v>
       </c>
       <c r="C121" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>129</v>
+        <v>240</v>
+      </c>
+      <c r="B122" t="s">
+        <v>241</v>
       </c>
       <c r="C122" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>130</v>
+        <v>242</v>
+      </c>
+      <c r="B123" t="s">
+        <v>243</v>
       </c>
       <c r="C123" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>131</v>
+        <v>244</v>
+      </c>
+      <c r="B124" t="s">
+        <v>245</v>
       </c>
       <c r="C124" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>132</v>
+        <v>246</v>
+      </c>
+      <c r="B125" t="s">
+        <v>247</v>
       </c>
       <c r="C125" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>133</v>
+        <v>248</v>
+      </c>
+      <c r="B126" t="s">
+        <v>249</v>
       </c>
       <c r="C126" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>134</v>
+        <v>250</v>
+      </c>
+      <c r="B127" t="s">
+        <v>251</v>
       </c>
       <c r="C127" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>135</v>
+        <v>252</v>
+      </c>
+      <c r="B128" t="s">
+        <v>253</v>
       </c>
       <c r="C128" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>136</v>
+        <v>254</v>
+      </c>
+      <c r="B129" t="s">
+        <v>255</v>
       </c>
       <c r="C129" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1898,29 +2631,29 @@
   <dimension ref="A1:DX1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="DV17" sqref="DV17"/>
+      <selection activeCell="DQ15" sqref="DQ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -1929,364 +2662,364 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="N1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="O1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="P1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="Q1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="R1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="S1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="T1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="U1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="V1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="W1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="X1" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="Y1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="Z1" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="AA1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="AB1" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="AC1" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="AD1" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="AE1" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="AF1" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="AG1" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="AH1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="AI1" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="AJ1" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="AK1" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="AL1" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="AM1" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="AN1" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="AO1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="AP1" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="AQ1" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="AR1" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="AS1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="AT1" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="AU1" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="AV1" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="AW1" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="AX1" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="AY1" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="AZ1" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="BA1" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="BB1" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="BC1" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="BD1" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="BE1" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="BF1" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="BG1" t="s">
-        <v>67</v>
+        <v>120</v>
       </c>
       <c r="BH1" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="BI1" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="BJ1" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="BK1" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="BL1" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="BM1" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="BN1" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="BO1" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="BP1" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="BQ1" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="BR1" t="s">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="BS1" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="BT1" t="s">
-        <v>80</v>
+        <v>146</v>
       </c>
       <c r="BU1" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="BV1" t="s">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="BW1" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="BX1" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="BY1" t="s">
-        <v>85</v>
+        <v>156</v>
       </c>
       <c r="BZ1" t="s">
-        <v>86</v>
+        <v>158</v>
       </c>
       <c r="CA1" t="s">
-        <v>87</v>
+        <v>160</v>
       </c>
       <c r="CB1" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="CC1" t="s">
-        <v>89</v>
+        <v>164</v>
       </c>
       <c r="CD1" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="CE1" t="s">
-        <v>91</v>
+        <v>168</v>
       </c>
       <c r="CF1" t="s">
-        <v>92</v>
+        <v>170</v>
       </c>
       <c r="CG1" t="s">
-        <v>93</v>
+        <v>172</v>
       </c>
       <c r="CH1" t="s">
-        <v>94</v>
+        <v>174</v>
       </c>
       <c r="CI1" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="CJ1" t="s">
-        <v>96</v>
+        <v>178</v>
       </c>
       <c r="CK1" t="s">
-        <v>97</v>
+        <v>180</v>
       </c>
       <c r="CL1" t="s">
-        <v>98</v>
+        <v>182</v>
       </c>
       <c r="CM1" t="s">
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="CN1" t="s">
-        <v>100</v>
+        <v>186</v>
       </c>
       <c r="CO1" t="s">
-        <v>101</v>
+        <v>188</v>
       </c>
       <c r="CP1" t="s">
-        <v>102</v>
+        <v>190</v>
       </c>
       <c r="CQ1" t="s">
-        <v>103</v>
+        <v>192</v>
       </c>
       <c r="CR1" t="s">
-        <v>104</v>
+        <v>194</v>
       </c>
       <c r="CS1" t="s">
-        <v>105</v>
+        <v>196</v>
       </c>
       <c r="CT1" t="s">
-        <v>106</v>
+        <v>198</v>
       </c>
       <c r="CU1" t="s">
-        <v>107</v>
+        <v>200</v>
       </c>
       <c r="CV1" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="CW1" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="CX1" t="s">
-        <v>110</v>
+        <v>206</v>
       </c>
       <c r="CY1" t="s">
-        <v>111</v>
+        <v>208</v>
       </c>
       <c r="CZ1" t="s">
-        <v>112</v>
+        <v>210</v>
       </c>
       <c r="DA1" t="s">
-        <v>113</v>
+        <v>212</v>
       </c>
       <c r="DB1" t="s">
-        <v>114</v>
+        <v>214</v>
       </c>
       <c r="DC1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="DD1" t="s">
-        <v>116</v>
+        <v>13</v>
       </c>
       <c r="DE1" t="s">
-        <v>117</v>
+        <v>216</v>
       </c>
       <c r="DF1" t="s">
-        <v>118</v>
+        <v>218</v>
       </c>
       <c r="DG1" t="s">
-        <v>119</v>
+        <v>220</v>
       </c>
       <c r="DH1" t="s">
-        <v>120</v>
+        <v>222</v>
       </c>
       <c r="DI1" t="s">
-        <v>121</v>
+        <v>224</v>
       </c>
       <c r="DJ1" t="s">
-        <v>122</v>
+        <v>226</v>
       </c>
       <c r="DK1" t="s">
-        <v>123</v>
+        <v>228</v>
       </c>
       <c r="DL1" t="s">
-        <v>124</v>
+        <v>230</v>
       </c>
       <c r="DM1" t="s">
-        <v>125</v>
+        <v>232</v>
       </c>
       <c r="DN1" t="s">
-        <v>126</v>
+        <v>234</v>
       </c>
       <c r="DO1" t="s">
-        <v>127</v>
+        <v>236</v>
       </c>
       <c r="DP1" t="s">
-        <v>128</v>
+        <v>238</v>
       </c>
       <c r="DQ1" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
       <c r="DR1" t="s">
-        <v>130</v>
+        <v>242</v>
       </c>
       <c r="DS1" t="s">
-        <v>131</v>
+        <v>244</v>
       </c>
       <c r="DT1" t="s">
-        <v>132</v>
+        <v>246</v>
       </c>
       <c r="DU1" t="s">
-        <v>133</v>
+        <v>248</v>
       </c>
       <c r="DV1" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="DW1" t="s">
-        <v>135</v>
+        <v>252</v>
       </c>
       <c r="DX1" t="s">
-        <v>136</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove onderstespronggewrich, but replace it with ankle for the model
</commit_message>
<xml_diff>
--- a/public/web_model/template.xlsx
+++ b/public/web_model/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\stage\CRISP\public\web_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84D21D6-B2F5-490D-A49C-9AE0B30391E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD7F48D-2746-4988-B32B-40A8B061C668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{28EB074A-B6E7-4FF4-9E0E-6C4DA293FACA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="272">
   <si>
     <t>MCV</t>
   </si>
@@ -69,18 +69,6 @@
     <t>ACPA</t>
   </si>
   <si>
-    <t>s_onderste_spronggewricht_left</t>
-  </si>
-  <si>
-    <t>s_onderste_spronggewricht_right</t>
-  </si>
-  <si>
-    <t>t_onderste_spronggewricht_left</t>
-  </si>
-  <si>
-    <t>t_onderste_spronggewricht_right</t>
-  </si>
-  <si>
     <t>Column</t>
   </si>
   <si>
@@ -805,13 +793,73 @@
   </si>
   <si>
     <t>Tender Wrist Right </t>
+  </si>
+  <si>
+    <t>t_mtp1_left </t>
+  </si>
+  <si>
+    <t>t_mtp1_right </t>
+  </si>
+  <si>
+    <t>t_mtp2_left </t>
+  </si>
+  <si>
+    <t>t_mtp2_right </t>
+  </si>
+  <si>
+    <t>stmtp3_left </t>
+  </si>
+  <si>
+    <t>t_mtp3_right </t>
+  </si>
+  <si>
+    <t>t_mtp4_left </t>
+  </si>
+  <si>
+    <t>t_mtp4_right </t>
+  </si>
+  <si>
+    <t>t_mtp5_left </t>
+  </si>
+  <si>
+    <t>t_mtp5_right </t>
+  </si>
+  <si>
+    <t>Tender Metatarsophalangeal I Left  </t>
+  </si>
+  <si>
+    <t>Tender Metatarsophalangeal I Right </t>
+  </si>
+  <si>
+    <t>Tender Metatarsophalangeal II Left  </t>
+  </si>
+  <si>
+    <t>Tender Metatarsophalangeal II Right </t>
+  </si>
+  <si>
+    <t>Tender Metatarsophalangeal III Left  </t>
+  </si>
+  <si>
+    <t>Tender Metatarsophalangeal III Right </t>
+  </si>
+  <si>
+    <t>Tender Metatarsophalangeal IV Left  </t>
+  </si>
+  <si>
+    <t>Tender Metatarsophalangeal IV Right </t>
+  </si>
+  <si>
+    <t>Tender Metatarsophalangeal V Left  </t>
+  </si>
+  <si>
+    <t>Tender Metatarsophalangeal V Right </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,19 +887,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -870,7 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1205,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60817267-BD25-47AD-969D-C9A5ECED4CFF}">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A129"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,16 +1268,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1236,10 +1285,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1247,10 +1296,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1258,7 +1307,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1266,10 +1315,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1277,7 +1326,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1285,10 +1334,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1296,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1304,10 +1353,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1315,10 +1364,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1326,421 +1375,425 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1751,7 +1804,7 @@
         <v>101</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1762,7 +1815,7 @@
         <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1773,7 +1826,7 @@
         <v>105</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1784,7 +1837,7 @@
         <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1795,7 +1848,7 @@
         <v>109</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1806,7 +1859,7 @@
         <v>111</v>
       </c>
       <c r="C55" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1817,7 +1870,7 @@
         <v>113</v>
       </c>
       <c r="C56" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1828,7 +1881,7 @@
         <v>115</v>
       </c>
       <c r="C57" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1839,7 +1892,7 @@
         <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1850,7 +1903,7 @@
         <v>119</v>
       </c>
       <c r="C59" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1861,7 +1914,7 @@
         <v>121</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1872,7 +1925,7 @@
         <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1883,7 +1936,7 @@
         <v>125</v>
       </c>
       <c r="C62" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1894,7 +1947,7 @@
         <v>127</v>
       </c>
       <c r="C63" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1905,7 +1958,7 @@
         <v>129</v>
       </c>
       <c r="C64" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1916,7 +1969,7 @@
         <v>131</v>
       </c>
       <c r="C65" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1927,7 +1980,7 @@
         <v>133</v>
       </c>
       <c r="C66" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1938,7 +1991,7 @@
         <v>135</v>
       </c>
       <c r="C67" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1949,7 +2002,7 @@
         <v>137</v>
       </c>
       <c r="C68" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1960,7 +2013,7 @@
         <v>139</v>
       </c>
       <c r="C69" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1971,7 +2024,7 @@
         <v>141</v>
       </c>
       <c r="C70" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1982,7 +2035,7 @@
         <v>143</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1993,7 +2046,7 @@
         <v>145</v>
       </c>
       <c r="C72" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2004,7 +2057,7 @@
         <v>147</v>
       </c>
       <c r="C73" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2015,7 +2068,7 @@
         <v>149</v>
       </c>
       <c r="C74" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,7 +2079,7 @@
         <v>151</v>
       </c>
       <c r="C75" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2037,7 +2090,7 @@
         <v>153</v>
       </c>
       <c r="C76" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2048,7 +2101,7 @@
         <v>155</v>
       </c>
       <c r="C77" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2059,7 +2112,7 @@
         <v>157</v>
       </c>
       <c r="C78" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2070,7 +2123,7 @@
         <v>159</v>
       </c>
       <c r="C79" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2081,7 +2134,7 @@
         <v>161</v>
       </c>
       <c r="C80" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2092,7 +2145,7 @@
         <v>163</v>
       </c>
       <c r="C81" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2103,7 +2156,7 @@
         <v>165</v>
       </c>
       <c r="C82" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2114,7 +2167,7 @@
         <v>167</v>
       </c>
       <c r="C83" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2125,7 +2178,7 @@
         <v>169</v>
       </c>
       <c r="C84" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,7 +2189,7 @@
         <v>171</v>
       </c>
       <c r="C85" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2147,7 +2200,7 @@
         <v>173</v>
       </c>
       <c r="C86" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2158,7 +2211,7 @@
         <v>175</v>
       </c>
       <c r="C87" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2169,7 +2222,7 @@
         <v>177</v>
       </c>
       <c r="C88" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -2180,7 +2233,7 @@
         <v>179</v>
       </c>
       <c r="C89" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2191,7 +2244,7 @@
         <v>181</v>
       </c>
       <c r="C90" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2202,7 +2255,7 @@
         <v>183</v>
       </c>
       <c r="C91" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2213,7 +2266,7 @@
         <v>185</v>
       </c>
       <c r="C92" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,7 +2277,7 @@
         <v>187</v>
       </c>
       <c r="C93" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2235,7 +2288,7 @@
         <v>189</v>
       </c>
       <c r="C94" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2246,7 +2299,7 @@
         <v>191</v>
       </c>
       <c r="C95" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2257,7 +2310,7 @@
         <v>193</v>
       </c>
       <c r="C96" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,7 +2321,7 @@
         <v>195</v>
       </c>
       <c r="C97" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2279,7 +2332,7 @@
         <v>197</v>
       </c>
       <c r="C98" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,7 +2343,7 @@
         <v>199</v>
       </c>
       <c r="C99" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2301,7 +2354,7 @@
         <v>201</v>
       </c>
       <c r="C100" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2312,7 +2365,7 @@
         <v>203</v>
       </c>
       <c r="C101" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,7 +2376,7 @@
         <v>205</v>
       </c>
       <c r="C102" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2387,7 @@
         <v>207</v>
       </c>
       <c r="C103" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,7 +2398,7 @@
         <v>209</v>
       </c>
       <c r="C104" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,267 +2409,337 @@
         <v>211</v>
       </c>
       <c r="C105" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>212</v>
-      </c>
-      <c r="B106" t="s">
-        <v>213</v>
-      </c>
-      <c r="C106" t="s">
-        <v>22</v>
+      <c r="A106" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>214</v>
-      </c>
-      <c r="B107" t="s">
-        <v>215</v>
-      </c>
-      <c r="C107" t="s">
-        <v>22</v>
+      <c r="A107" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>12</v>
-      </c>
-      <c r="B108" s="3"/>
-      <c r="C108" t="s">
-        <v>22</v>
+      <c r="A108" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>13</v>
-      </c>
-      <c r="B109" s="3"/>
-      <c r="C109" t="s">
-        <v>22</v>
+      <c r="A109" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>216</v>
-      </c>
-      <c r="B110" t="s">
-        <v>217</v>
-      </c>
-      <c r="C110" t="s">
-        <v>22</v>
+      <c r="A110" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>218</v>
-      </c>
-      <c r="B111" t="s">
-        <v>219</v>
-      </c>
-      <c r="C111" t="s">
-        <v>22</v>
+      <c r="A111" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>220</v>
-      </c>
-      <c r="B112" t="s">
-        <v>221</v>
-      </c>
-      <c r="C112" t="s">
-        <v>22</v>
+      <c r="A112" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>222</v>
-      </c>
-      <c r="B113" t="s">
-        <v>223</v>
-      </c>
-      <c r="C113" t="s">
-        <v>22</v>
+      <c r="A113" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>224</v>
-      </c>
-      <c r="B114" t="s">
-        <v>225</v>
-      </c>
-      <c r="C114" t="s">
-        <v>22</v>
+      <c r="A114" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>226</v>
-      </c>
-      <c r="B115" t="s">
-        <v>227</v>
-      </c>
-      <c r="C115" t="s">
-        <v>22</v>
+      <c r="A115" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B116" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C116" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="B117" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="C117" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="B118" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="C118" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B119" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="C119" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="B120" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="C120" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="B121" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="C121" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="B122" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="C122" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B123" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="C123" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="B124" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="C124" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B125" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="C125" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="B126" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="C126" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B127" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="C127" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B128" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="C128" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B129" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="C129" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>240</v>
+      </c>
+      <c r="B130" t="s">
+        <v>241</v>
+      </c>
+      <c r="C130" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>242</v>
+      </c>
+      <c r="B131" t="s">
+        <v>243</v>
+      </c>
+      <c r="C131" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>244</v>
+      </c>
+      <c r="B132" t="s">
+        <v>245</v>
+      </c>
+      <c r="C132" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>246</v>
+      </c>
+      <c r="B133" t="s">
+        <v>247</v>
+      </c>
+      <c r="C133" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>248</v>
+      </c>
+      <c r="B134" t="s">
+        <v>249</v>
+      </c>
+      <c r="C134" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>250</v>
+      </c>
+      <c r="B135" t="s">
+        <v>251</v>
+      </c>
+      <c r="C135" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2628,15 +2751,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1770448-8847-4091-BEBE-01B00610DEBD}">
-  <dimension ref="A1:DX1"/>
+  <dimension ref="A1:ED117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="DQ15" sqref="DQ15"/>
+    <sheetView tabSelected="1" topLeftCell="DI1" workbookViewId="0">
+      <selection activeCell="EE1" sqref="EE1:EI1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2668,118 +2794,118 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>40</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>44</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>48</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>50</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>52</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>58</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>60</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>62</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>64</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>66</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>68</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>72</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>74</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>76</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>78</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>80</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>82</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>84</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>86</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>88</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>90</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>92</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>94</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>96</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>98</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>11</v>
       </c>
       <c r="AW1" t="s">
         <v>100</v>
@@ -2949,78 +3075,126 @@
       <c r="CZ1" t="s">
         <v>210</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DA1" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="DB1" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="DC1" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="DD1" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="DE1" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="DF1" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="DG1" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="DH1" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="DI1" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="DJ1" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="DK1" t="s">
         <v>212</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DL1" t="s">
         <v>214</v>
       </c>
-      <c r="DC1" t="s">
-        <v>12</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>13</v>
-      </c>
-      <c r="DE1" t="s">
+      <c r="DM1" t="s">
         <v>216</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DN1" t="s">
         <v>218</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DO1" t="s">
         <v>220</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DP1" t="s">
         <v>222</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DQ1" t="s">
         <v>224</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DR1" t="s">
         <v>226</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DS1" t="s">
         <v>228</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DT1" t="s">
         <v>230</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DU1" t="s">
         <v>232</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DV1" t="s">
         <v>234</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DW1" t="s">
         <v>236</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DX1" t="s">
         <v>238</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DY1" t="s">
         <v>240</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DZ1" t="s">
         <v>242</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="EA1" t="s">
         <v>244</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="EB1" t="s">
         <v>246</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="EC1" t="s">
         <v>248</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="ED1" t="s">
         <v>250</v>
       </c>
-      <c r="DW1" t="s">
-        <v>252</v>
-      </c>
-      <c r="DX1" t="s">
-        <v>254</v>
-      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="3"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="3"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>